<commit_message>
Actualizacion de estructura de  datos
</commit_message>
<xml_diff>
--- a/tp final/wordix/wordix/estructurasDatosWordix.xlsx
+++ b/tp final/wordix/wordix/estructurasDatosWordix.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{266CDDAB-E224-49BC-8F9C-699CFA840F67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="14880" windowHeight="7815"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EstructuraDatos" sheetId="1" r:id="rId1"/>
@@ -14,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="43">
   <si>
     <t>$coleccionPalabras=</t>
   </si>
@@ -62,13 +63,94 @@
   </si>
   <si>
     <t>¿Para qué se utiliza?: guarda las palabras que se pueden elegidas para jugar wordix</t>
+  </si>
+  <si>
+    <t>$coleccionPartidas</t>
+  </si>
+  <si>
+    <t>"partida"</t>
+  </si>
+  <si>
+    <t>"puntaje"</t>
+  </si>
+  <si>
+    <t>"jugador"</t>
+  </si>
+  <si>
+    <t>"intento"</t>
+  </si>
+  <si>
+    <t>"fede"</t>
+  </si>
+  <si>
+    <t>"palabra</t>
+  </si>
+  <si>
+    <t>"QUESO"</t>
+  </si>
+  <si>
+    <t>"No adivino la palabra"</t>
+  </si>
+  <si>
+    <t>"MUJER"</t>
+  </si>
+  <si>
+    <t>"joaquin"</t>
+  </si>
+  <si>
+    <t>"FUEGO"</t>
+  </si>
+  <si>
+    <t>"Adivino la palabra en 1 intento"</t>
+  </si>
+  <si>
+    <t>"CASAS"</t>
+  </si>
+  <si>
+    <t>"QUESO</t>
+  </si>
+  <si>
+    <t>"moni"</t>
+  </si>
+  <si>
+    <t>"Adivino la palabra en 6 intentos"</t>
+  </si>
+  <si>
+    <t>"Adivino la palabra en 2 intentos</t>
+  </si>
+  <si>
+    <t>"PIANO"</t>
+  </si>
+  <si>
+    <t>"Adivino la palabra en 4 intentos"</t>
+  </si>
+  <si>
+    <t>"MELON"</t>
+  </si>
+  <si>
+    <t>"CABRA"</t>
+  </si>
+  <si>
+    <t>"CEJAS"</t>
+  </si>
+  <si>
+    <t>"Adivino la palabra en 3 intentos"</t>
+  </si>
+  <si>
+    <t>"ABETO"</t>
+  </si>
+  <si>
+    <t>"Adivino la palabra en 2 intentos"</t>
+  </si>
+  <si>
+    <t>"VERDE"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -103,6 +185,20 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFD4D4D4"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -154,35 +250,50 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -220,7 +331,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -254,6 +365,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -288,9 +400,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -463,30 +576,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" customWidth="1"/>
-    <col min="7" max="7" width="12" customWidth="1"/>
+    <col min="1" max="1" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21" customWidth="1"/>
+    <col min="3" max="3" width="29.44140625" customWidth="1"/>
+    <col min="4" max="4" width="31.5546875" customWidth="1"/>
+    <col min="5" max="5" width="21.77734375" customWidth="1"/>
+    <col min="6" max="6" width="29.44140625" customWidth="1"/>
+    <col min="7" max="7" width="30.44140625" customWidth="1"/>
+    <col min="8" max="8" width="21.77734375" customWidth="1"/>
+    <col min="9" max="9" width="28.44140625" customWidth="1"/>
+    <col min="10" max="10" width="27.88671875" customWidth="1"/>
+    <col min="11" max="11" width="28.109375" customWidth="1"/>
+    <col min="12" max="12" width="22.6640625" customWidth="1"/>
+    <col min="13" max="14" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -512,7 +631,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
@@ -535,35 +654,333 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="8">
+        <v>0</v>
+      </c>
+      <c r="C15" s="8">
+        <v>1</v>
+      </c>
+      <c r="D15" s="8">
+        <v>2</v>
+      </c>
+      <c r="E15" s="8">
+        <v>3</v>
+      </c>
+      <c r="F15" s="8">
+        <v>4</v>
+      </c>
+      <c r="G15" s="8">
+        <v>5</v>
+      </c>
+      <c r="H15" s="8">
+        <v>6</v>
+      </c>
+      <c r="I15" s="8">
+        <v>7</v>
+      </c>
+      <c r="J15" s="8">
+        <v>8</v>
+      </c>
+      <c r="K15" s="8">
+        <v>9</v>
+      </c>
+      <c r="L15" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1</v>
+      </c>
+      <c r="C16" s="1">
+        <v>2</v>
+      </c>
+      <c r="D16" s="1">
+        <v>3</v>
+      </c>
+      <c r="E16" s="1">
+        <v>4</v>
+      </c>
+      <c r="F16" s="1">
+        <v>5</v>
+      </c>
+      <c r="G16" s="1">
+        <v>6</v>
+      </c>
+      <c r="H16" s="1">
+        <v>7</v>
+      </c>
+      <c r="I16" s="1">
+        <v>8</v>
+      </c>
+      <c r="J16" s="1">
+        <v>9</v>
+      </c>
+      <c r="K16" s="1">
+        <v>10</v>
+      </c>
+      <c r="L16" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1">
+        <v>0</v>
+      </c>
+      <c r="C19" s="1">
+        <v>16</v>
+      </c>
+      <c r="D19" s="1">
+        <v>20</v>
+      </c>
+      <c r="E19" s="1">
+        <v>0</v>
+      </c>
+      <c r="F19" s="1">
+        <v>6</v>
+      </c>
+      <c r="G19" s="1">
+        <v>10</v>
+      </c>
+      <c r="H19" s="1">
+        <v>0</v>
+      </c>
+      <c r="I19" s="1">
+        <v>10</v>
+      </c>
+      <c r="J19" s="1">
+        <v>12</v>
+      </c>
+      <c r="K19" s="1">
+        <v>15</v>
+      </c>
+      <c r="L19" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I21" s="7"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I22" s="7"/>
+      <c r="L22" s="9"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I23" s="7"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D24" s="9"/>
+      <c r="I24" s="7"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C25" s="9"/>
+      <c r="I25" s="7"/>
+      <c r="K25" s="9"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I26" s="7"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I27" s="7"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I28" s="7"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I29" s="7"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I30" s="7"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I31" s="7"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I32" s="7"/>
+    </row>
+    <row r="33" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I33" s="7"/>
+    </row>
+    <row r="34" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I34" s="7"/>
+    </row>
+    <row r="35" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I35" s="7"/>
+    </row>
+    <row r="36" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I36" s="7"/>
+    </row>
+    <row r="37" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I37" s="7"/>
+    </row>
+    <row r="38" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I38" s="7"/>
+    </row>
+    <row r="39" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I39" s="7"/>
+    </row>
+    <row r="40" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I40" s="7"/>
+    </row>
+    <row r="41" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I41" s="7"/>
+    </row>
+    <row r="42" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I42" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Agregué las especificaciones del arreglo estructurasDatosWordix.xlsx . Especifique el tipo de arreglo, los tipos de datos y que funcion cumple
</commit_message>
<xml_diff>
--- a/tp final/wordix/wordix/estructurasDatosWordix.xlsx
+++ b/tp final/wordix/wordix/estructurasDatosWordix.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{266CDDAB-E224-49BC-8F9C-699CFA840F67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896"/>
   </bookViews>
   <sheets>
     <sheet name="EstructuraDatos" sheetId="1" r:id="rId1"/>
@@ -15,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="46">
   <si>
     <t>$coleccionPalabras=</t>
   </si>
@@ -62,9 +61,6 @@
     <t>A continuación puede agregar el resto de las estructuras de datos</t>
   </si>
   <si>
-    <t>¿Para qué se utiliza?: guarda las palabras que se pueden elegidas para jugar wordix</t>
-  </si>
-  <si>
     <t>$coleccionPartidas</t>
   </si>
   <si>
@@ -144,12 +140,24 @@
   </si>
   <si>
     <t>"VERDE"</t>
+  </si>
+  <si>
+    <t>Tipo: Multidimensional. Indexado (los índices son numéricos) con arreglos asociativos</t>
+  </si>
+  <si>
+    <t>Tipos de datos: Almacena en cada posición un arreglo asociativo con claves String y valores String y Entero</t>
+  </si>
+  <si>
+    <t>¿Para qué se utiliza?: guardar las palabras que se pueden elegir para jugar wordix</t>
+  </si>
+  <si>
+    <t>¿Para qué se utiliza?: guardar cada una de las partidas jugadas con los datos relevantes de cada una</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -291,9 +299,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -331,9 +339,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -368,7 +376,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -403,7 +411,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -576,11 +584,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -671,7 +679,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
@@ -686,7 +694,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" s="8">
         <v>0</v>
@@ -724,7 +732,7 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16" s="1">
         <v>1</v>
@@ -762,83 +770,83 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="C17" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F17" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="G17" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H17" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I17" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="I17" s="1" t="s">
+      <c r="J17" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="J17" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="K17" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" s="1">
         <v>0</v>
@@ -876,40 +884,40 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
@@ -920,18 +928,30 @@
       <c r="L22" s="9"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B23" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="I23" s="7"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>42</v>
+      </c>
       <c r="D24" s="9"/>
       <c r="I24" s="7"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>43</v>
+      </c>
       <c r="C25" s="9"/>
       <c r="I25" s="7"/>
       <c r="K25" s="9"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>45</v>
+      </c>
       <c r="I26" s="7"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Agregué los arreglos de las vocales y las consonantes para calcular los puntajes
</commit_message>
<xml_diff>
--- a/tp final/wordix/wordix/estructurasDatosWordix.xlsx
+++ b/tp final/wordix/wordix/estructurasDatosWordix.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="78">
   <si>
     <t>$coleccionPalabras=</t>
   </si>
@@ -152,6 +152,102 @@
   </si>
   <si>
     <t>¿Para qué se utiliza?: guardar cada una de las partidas jugadas con los datos relevantes de cada una</t>
+  </si>
+  <si>
+    <t>$coleccionVocales</t>
+  </si>
+  <si>
+    <t>"A"</t>
+  </si>
+  <si>
+    <t>"E"</t>
+  </si>
+  <si>
+    <t>"I"</t>
+  </si>
+  <si>
+    <t>"O"</t>
+  </si>
+  <si>
+    <t>"U"</t>
+  </si>
+  <si>
+    <t>¿Para qué se utiliza?: guardar las vocales para ir calculando el puntaje en las partidas</t>
+  </si>
+  <si>
+    <t>$coleccionConsonant1</t>
+  </si>
+  <si>
+    <t>"B"</t>
+  </si>
+  <si>
+    <t>"C"</t>
+  </si>
+  <si>
+    <t>"D"</t>
+  </si>
+  <si>
+    <t>"F"</t>
+  </si>
+  <si>
+    <t>"G"</t>
+  </si>
+  <si>
+    <t>"H"</t>
+  </si>
+  <si>
+    <t>"J"</t>
+  </si>
+  <si>
+    <t>"K"</t>
+  </si>
+  <si>
+    <t>"L"</t>
+  </si>
+  <si>
+    <t>"M"</t>
+  </si>
+  <si>
+    <t>$coleccionConsonant2</t>
+  </si>
+  <si>
+    <t>"N"</t>
+  </si>
+  <si>
+    <t>"P"</t>
+  </si>
+  <si>
+    <t>"Q"</t>
+  </si>
+  <si>
+    <t>"R"</t>
+  </si>
+  <si>
+    <t>"S"</t>
+  </si>
+  <si>
+    <t>"T"</t>
+  </si>
+  <si>
+    <t>"V"</t>
+  </si>
+  <si>
+    <t>"W"</t>
+  </si>
+  <si>
+    <t>"X"</t>
+  </si>
+  <si>
+    <t>"Y"</t>
+  </si>
+  <si>
+    <t>"Z"</t>
+  </si>
+  <si>
+    <t>¿Para qué se utiliza?: guardar las consonantes desde la B hasta la M para ir calculando el puntaje en las partidas</t>
+  </si>
+  <si>
+    <t>¿Para qué se utiliza?: guardar las consonantes desde la N hasta la Z para ir calculando el puntaje en las partidas</t>
   </si>
 </sst>
 </file>
@@ -585,15 +681,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L42"/>
+  <dimension ref="A1:L53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.109375" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
     <col min="3" max="3" width="29.44140625" customWidth="1"/>
     <col min="4" max="4" width="31.5546875" customWidth="1"/>
@@ -961,46 +1057,261 @@
       <c r="I28" s="7"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>46</v>
+      </c>
+      <c r="B29" s="2">
+        <v>0</v>
+      </c>
+      <c r="C29" s="2">
+        <v>1</v>
+      </c>
+      <c r="D29" s="2">
+        <v>2</v>
+      </c>
+      <c r="E29" s="2">
+        <v>3</v>
+      </c>
+      <c r="F29" s="2">
+        <v>4</v>
+      </c>
       <c r="I29" s="7"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B30" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="I30" s="7"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="I31" s="7"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B32" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="I32" s="7"/>
     </row>
-    <row r="33" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>8</v>
+      </c>
       <c r="I33" s="7"/>
     </row>
-    <row r="34" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>7</v>
+      </c>
       <c r="I34" s="7"/>
     </row>
-    <row r="35" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
+        <v>52</v>
+      </c>
       <c r="I35" s="7"/>
     </row>
-    <row r="36" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="I36" s="7"/>
     </row>
-    <row r="37" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="I37" s="7"/>
     </row>
-    <row r="38" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I38" s="7"/>
-    </row>
-    <row r="39" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I39" s="7"/>
-    </row>
-    <row r="40" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>53</v>
+      </c>
+      <c r="B38" s="2">
+        <v>0</v>
+      </c>
+      <c r="C38" s="2">
+        <v>1</v>
+      </c>
+      <c r="D38" s="2">
+        <v>2</v>
+      </c>
+      <c r="E38" s="2">
+        <v>3</v>
+      </c>
+      <c r="F38" s="2">
+        <v>4</v>
+      </c>
+      <c r="G38" s="2">
+        <v>5</v>
+      </c>
+      <c r="H38" s="2">
+        <v>6</v>
+      </c>
+      <c r="I38" s="2">
+        <v>7</v>
+      </c>
+      <c r="J38" s="2">
+        <v>8</v>
+      </c>
+      <c r="K38" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B39" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="I40" s="7"/>
     </row>
-    <row r="41" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B41" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="I41" s="7"/>
     </row>
-    <row r="42" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B42" t="s">
+        <v>8</v>
+      </c>
       <c r="I42" s="7"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B43" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B44" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>64</v>
+      </c>
+      <c r="B47" s="2">
+        <v>0</v>
+      </c>
+      <c r="C47" s="2">
+        <v>1</v>
+      </c>
+      <c r="D47" s="2">
+        <v>2</v>
+      </c>
+      <c r="E47" s="2">
+        <v>3</v>
+      </c>
+      <c r="F47" s="2">
+        <v>4</v>
+      </c>
+      <c r="G47" s="2">
+        <v>5</v>
+      </c>
+      <c r="H47" s="2">
+        <v>6</v>
+      </c>
+      <c r="I47" s="2">
+        <v>7</v>
+      </c>
+      <c r="J47" s="2">
+        <v>8</v>
+      </c>
+      <c r="K47" s="2">
+        <v>9</v>
+      </c>
+      <c r="L47" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B48" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J48" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="K48" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="L48" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B50" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B51" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B52" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B53" t="s">
+        <v>77</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>